<commit_message>
update to color scheme
- barrier island species are now included in MP_2023_color_ramp
</commit_message>
<xml_diff>
--- a/MP_2023_color_ramp.xlsx
+++ b/MP_2023_color_ramp.xlsx
@@ -5,27 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\Coastal Hydro Dropbox\Madeline Foster-Martinez\MRF_LAVegMod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\Documents\GitHub\ICM_LAVegMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF0BD70-D397-4316-8185-D3EB148C7CC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC835F25-731D-46B1-A487-C7EDB9585C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="1935" windowWidth="17325" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5748" yWindow="5484" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
   <si>
     <t>Symbol</t>
   </si>
@@ -271,6 +279,48 @@
   </si>
   <si>
     <t>BAREGRND_NEW</t>
+  </si>
+  <si>
+    <t>BAHABI</t>
+  </si>
+  <si>
+    <t>DISPBI</t>
+  </si>
+  <si>
+    <t>PAAM2</t>
+  </si>
+  <si>
+    <t>SOSE</t>
+  </si>
+  <si>
+    <t>SPPABI</t>
+  </si>
+  <si>
+    <t>SPVI3</t>
+  </si>
+  <si>
+    <t>STHE9</t>
+  </si>
+  <si>
+    <t>UNPA</t>
+  </si>
+  <si>
+    <t>Seaoats</t>
+  </si>
+  <si>
+    <t>Seashore dropseed</t>
+  </si>
+  <si>
+    <t>Seaside goldenrod</t>
+  </si>
+  <si>
+    <t>amberique-bean</t>
+  </si>
+  <si>
+    <t>Bitter panicgrass</t>
+  </si>
+  <si>
+    <t>Eastern baccharis</t>
   </si>
 </sst>
 </file>
@@ -304,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,6 +592,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7F4413"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF660033"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99004C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF007F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66B2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCE5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -603,6 +701,15 @@
     <xf numFmtId="0" fontId="3" fillId="39" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,16 +719,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCE5"/>
+      <color rgb="FFFF99CC"/>
+      <color rgb="FFFF66B2"/>
+      <color rgb="FFFF007F"/>
+      <color rgb="FFFF3399"/>
+      <color rgb="FFCC0066"/>
+      <color rgb="FF99004C"/>
+      <color rgb="FF660033"/>
       <color rgb="FF7F4413"/>
       <color rgb="FF67370F"/>
-      <color rgb="FFE1FF8B"/>
-      <color rgb="FF7DD5A9"/>
-      <color rgb="FF3DB97B"/>
-      <color rgb="FF339966"/>
-      <color rgb="FF899735"/>
-      <color rgb="FF677228"/>
-      <color rgb="FF7BB800"/>
-      <color rgb="FF669900"/>
     </mruColors>
   </colors>
   <extLst>
@@ -898,18 +1005,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -932,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>58</v>
       </c>
@@ -953,7 +1060,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -974,7 +1081,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -995,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>81</v>
       </c>
@@ -1011,7 +1118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>21</v>
       </c>
@@ -1032,7 +1139,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>24</v>
       </c>
@@ -1053,7 +1160,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>25</v>
       </c>
@@ -1074,7 +1181,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>19</v>
       </c>
@@ -1095,7 +1202,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20</v>
       </c>
@@ -1116,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>22</v>
       </c>
@@ -1137,7 +1244,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>26</v>
       </c>
@@ -1158,7 +1265,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>29</v>
       </c>
@@ -1179,7 +1286,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>31</v>
       </c>
@@ -1200,7 +1307,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>33</v>
       </c>
@@ -1221,7 +1328,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>37</v>
       </c>
@@ -1242,7 +1349,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>80</v>
       </c>
@@ -1258,7 +1365,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1267,7 +1374,7 @@
       </c>
       <c r="D18" s="42"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>38</v>
       </c>
@@ -1288,7 +1395,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>34</v>
       </c>
@@ -1309,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>36</v>
       </c>
@@ -1330,7 +1437,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1348,7 +1455,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>35</v>
       </c>
@@ -1369,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>42</v>
       </c>
@@ -1390,7 +1497,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>43</v>
       </c>
@@ -1411,7 +1518,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>48</v>
       </c>
@@ -1432,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>45</v>
       </c>
@@ -1453,7 +1560,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>46</v>
       </c>
@@ -1474,7 +1581,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>41</v>
       </c>
@@ -1495,7 +1602,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>39</v>
       </c>
@@ -1516,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>44</v>
       </c>
@@ -1537,7 +1644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>40</v>
       </c>
@@ -1558,7 +1665,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>49</v>
       </c>
@@ -1579,7 +1686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>47</v>
       </c>
@@ -1600,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>51</v>
       </c>
@@ -1621,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>50</v>
       </c>
@@ -1642,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>55</v>
       </c>
@@ -1663,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>52</v>
       </c>
@@ -1684,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>53</v>
       </c>
@@ -1705,7 +1812,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>54</v>
       </c>
@@ -1726,21 +1833,165 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="43"/>
+      <c r="E41" s="42">
+        <v>102</v>
+      </c>
+      <c r="F41" s="42">
+        <v>0</v>
+      </c>
+      <c r="G41" s="42">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="44"/>
+      <c r="E42" s="42">
+        <v>153</v>
+      </c>
+      <c r="F42" s="42">
+        <v>0</v>
+      </c>
+      <c r="G42" s="42">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="45"/>
+      <c r="E43" s="42">
+        <v>204</v>
+      </c>
+      <c r="F43" s="42">
+        <v>0</v>
+      </c>
+      <c r="G43" s="42">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="47"/>
+      <c r="E44" s="42">
+        <v>255</v>
+      </c>
+      <c r="F44" s="42">
+        <v>0</v>
+      </c>
+      <c r="G44" s="42">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="46"/>
+      <c r="E45" s="42">
+        <v>255</v>
+      </c>
+      <c r="F45" s="42">
+        <v>51</v>
+      </c>
+      <c r="G45" s="42">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="48"/>
+      <c r="E46" s="42">
+        <v>255</v>
+      </c>
+      <c r="F46" s="42">
+        <v>102</v>
+      </c>
+      <c r="G46" s="42">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="49"/>
+      <c r="E47" s="42">
+        <v>255</v>
+      </c>
+      <c r="F47" s="42">
+        <v>153</v>
+      </c>
+      <c r="G47" s="42">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="50"/>
+      <c r="E48" s="42">
+        <v>255</v>
+      </c>
+      <c r="F48" s="42">
+        <v>204</v>
+      </c>
+      <c r="G48" s="42">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="2">
-        <v>0</v>
-      </c>
-      <c r="F44" s="2">
-        <v>255</v>
-      </c>
-      <c r="G44" s="2">
+      <c r="D49" s="5"/>
+      <c r="E49" s="2">
+        <v>0</v>
+      </c>
+      <c r="F49" s="2">
+        <v>255</v>
+      </c>
+      <c r="G49" s="2">
         <v>255</v>
       </c>
     </row>

</xml_diff>